<commit_message>
Dataset sorting fix + new training models and tweaks
</commit_message>
<xml_diff>
--- a/machinelearning/posts_clf/execution_results.xlsx
+++ b/machinelearning/posts_clf/execution_results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,12 +435,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0:00:07.620528</t>
+          <t>0:00:07.418083</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0:00:00.082799</t>
+          <t>0:00:00.082776</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -454,6 +454,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.968993219791301</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.947845014022408</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.7424400604795162, 'recall': 0.8383536585365854, 'f1-score': 0.7874871129100004, 'support': 49200}, 'depression': {'precision': 0.9879939494215115, 'recall': 0.978604068352144, 'f1-score': 0.9832765920365869, 'support': 668772}, 'accuracy': 0.968993219791301, 'macro avg': {'precision': 0.8652170049505139, 'recall': 0.9084788634443647, 'f1-score': 0.8853818524732937, 'support': 717972}, 'weighted avg': {'precision': 0.9711670378762896, 'recall': 0.968993219791301, 'f1-score': 0.9698598538169515, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9267322728498247, 'recall': 0.8383536585365854, 'f1-score': 0.8803303880138301, 'support': 49200}, 'depression': {'precision': 0.9533562065628574, 'recall': 0.980333266993541, 'f1-score': 0.9666565571869481, 'support': 165813}, 'accuracy': 0.947845014022408, 'macro avg': {'precision': 0.9400442397063411, 'recall': 0.9093434627650632, 'f1-score': 0.9234934726003892, 'support': 215013}, 'weighted avg': {'precision': 0.9472640282355879, 'recall': 0.947845014022408, 'f1-score': 0.9469031119379752, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0:00:06.692001</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0:00:00.076772</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>BOW with (1-1) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.6912205489907685</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.7550427183472628</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.1673410036757474, 'recall': 0.8818292682926829, 'f1-score': 0.28130075502403823, 'support': 49200}, 'depression': {'precision': 0.9873251872118246, 'recall': 0.6771979090033674, 'f1-score': 0.8033707117750518, 'support': 668772}, 'accuracy': 0.6912205489907685, 'macro avg': {'precision': 0.577333095443786, 'recall': 0.7795135886480251, 'f1-score': 0.542335733399545, 'support': 717972}, 'weighted avg': {'precision': 0.9311346646984466, 'recall': 0.6912205489907685, 'f1-score': 0.7675951636030481, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.48077924668387984, 'recall': 0.8818292682926829, 'f1-score': 0.6222846938848688, 'support': 49200}, 'depression': {'precision': 0.9534030070849229, 'recall': 0.7174226387557068, 'f1-score': 0.8187483868747527, 'support': 165813}, 'accuracy': 0.7550427183472628, 'macro avg': {'precision': 0.7170911268844014, 'recall': 0.7996259535241949, 'f1-score': 0.7205165403798108, 'support': 215013}, 'weighted avg': {'precision': 0.8452556438476706, 'recall': 0.7550427183472628, 'f1-score': 0.7737929018803463, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0:00:09.311335</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0:00:00.187498</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>BOW with (1-1) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.01, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -463,84 +545,166 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0.9807067685090783</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.92799040058043</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9457278321396146, 'recall': 0.7621951219512195, 'f1-score': 0.8441003016251745, 'support': 49200}, 'depression': {'precision': 0.9827515037150607, 'recall': 0.9967821619326168, 'f1-score': 0.9897171091506742, 'support': 668772}, 'accuracy': 0.9807067685090783, 'macro avg': {'precision': 0.9642396679273377, 'recall': 0.8794886419419181, 'f1-score': 0.9169087053879243, 'support': 717972}, 'weighted avg': {'precision': 0.9802144066673877, 'recall': 0.9807067685090783, 'f1-score': 0.979738520946323, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9829270388724971, 'recall': 0.6974186991869918, 'f1-score': 0.8159174404641596, 'support': 49200}, 'depression': {'precision': 0.9173422022831254, 'recall': 0.9964055894290557, 'f1-score': 0.9552407080311173, 'support': 165813}, 'accuracy': 0.92799040058043, 'macro avg': {'precision': 0.9501346205778112, 'recall': 0.8469121443080238, 'f1-score': 0.8855790742476384, 'support': 215013}, 'weighted avg': {'precision': 0.9323495458400131, 'recall': 0.92799040058043, 'f1-score': 0.923360287943521, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0:00:25.139658</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0:00:00.452792</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="C5" t="n">
+        <v>0.9803933858144885</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9275346141861189</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9449666810246535, 'recall': 0.7580284552845529, 'f1-score': 0.8412374389569964, 'support': 49200}, 'depression': {'precision': 0.9824540718196624, 'recall': 0.9967522563743697, 'f1-score': 0.9895515176166446, 'support': 668772}, 'accuracy': 0.9803933858144885, 'macro avg': {'precision': 0.963710376422158, 'recall': 0.8773903558294613, 'f1-score': 0.9153944782868205, 'support': 717972}, 'weighted avg': {'precision': 0.9798851977868108, 'recall': 0.9803933858144885, 'f1-score': 0.9793880952686217, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9832676882385073, 'recall': 0.6951422764227643, 'f1-score': 0.8144743579057667, 'support': 49200}, 'depression': {'precision': 0.9167785607279587, 'recall': 0.9964900218921315, 'f1-score': 0.9549738038336276, 'support': 165813}, 'accuracy': 0.9275346141861189, 'macro avg': {'precision': 0.950023124483233, 'recall': 0.8458161491574478, 'f1-score': 0.8847240808696972, 'support': 215013}, 'weighted avg': {'precision': 0.9319928271840289, 'recall': 0.9275346141861189, 'f1-score': 0.9228242466456866, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0:00:23.909848</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0:00:00.409903</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>BOW with (1-1) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>MultinomialNB(alpha=0.1, class_prior=None, fit_prior=True)</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C6" t="n">
         <v>0.9686645161649758</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D6" t="n">
         <v>0.9327156962602261</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.7752102572559367, 'recall': 0.764369918699187, 'f1-score': 0.7697519240216146, 'support': 49200}, 'depression': {'precision': 0.9826830579870344, 'recall': 0.9836939943657929, 'f1-score': 0.9831882663095787, 'support': 668772}, 'accuracy': 0.9686645161649758, 'macro avg': {'precision': 0.8789466576214855, 'recall': 0.8740319565324899, 'f1-score': 0.8764700951655966, 'support': 717972}, 'weighted avg': {'precision': 0.9684657043911142, 'recall': 0.9686645161649758, 'f1-score': 0.9685622529823628, 'support': 717972}}</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.9290037301450063, 'recall': 0.764369918699187, 'f1-score': 0.838683779172846, 'support': 49200}, 'depression': {'precision': 0.9335766507001582, 'recall': 0.9826672215085669, 'f1-score': 0.9574931319690315, 'support': 165813}, 'accuracy': 0.9327156962602261, 'macro avg': {'precision': 0.9312901904225822, 'recall': 0.873518570103877, 'f1-score': 0.8980884555709387, 'support': 215013}, 'weighted avg': {'precision': 0.932530259592116, 'recall': 0.9327156962602261, 'f1-score': 0.9303067750623685, 'support': 215013}}</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0:00:09.807564</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0:00:00.119681</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0:00:07.481753</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0:00:00.103701</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>BOW with (1-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9583994919021912</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9448451954067894</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.6469667021438346, 'recall': 0.8648577235772358, 'f1-score': 0.7402104896929634, 'support': 49200}, 'depression': {'precision': 0.989805305718167, 'recall': 0.9652811421530806, 'f1-score': 0.9773894111466236, 'support': 668772}, 'accuracy': 0.9583994919021912, 'macro avg': {'precision': 0.8183860039310008, 'recall': 0.9150694328651582, 'f1-score': 0.8587999504197935, 'support': 717972}, 'weighted avg': {'precision': 0.966311827844577, 'recall': 0.9583994919021912, 'f1-score': 0.9611364055481878, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.8909151818429263, 'recall': 0.8648577235772358, 'f1-score': 0.8776930930992874, 'support': 49200}, 'depression': {'precision': 0.9602456173917203, 'recall': 0.9685790619553353, 'f1-score': 0.9643943374416406, 'support': 165813}, 'accuracy': 0.9448451954067894, 'macro avg': {'precision': 0.9255803996173233, 'recall': 0.9167183927662855, 'f1-score': 0.921043715270464, 'support': 215013}, 'weighted avg': {'precision': 0.9443811932452704, 'recall': 0.9448451954067894, 'f1-score': 0.9445550662271383, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0:00:07.780246</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0:00:00.095744</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>BOW with (1-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=0.1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6761196815474698</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7427922962797598</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.16133120037831628, 'recall': 0.8875609756097561, 'f1-score': 0.2730333601147955, 'support': 49200}, 'depression': {'precision': 0.9876324337859016, 'recall': 0.660564437506355, 'f1-score': 0.791646767992359, 'support': 668772}, 'accuracy': 0.6761196815474698, 'macro avg': {'precision': 0.5744818170821089, 'recall': 0.7740627065580555, 'f1-score': 0.5323400640535773, 'support': 717972}, 'weighted avg': {'precision': 0.9310090269070076, 'recall': 0.6761196815474698, 'f1-score': 0.7561080844955428, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.46734233029034983, 'recall': 0.8875609756097561, 'f1-score': 0.6122869621912661, 'support': 49200}, 'depression': {'precision': 0.954496849655354, 'recall': 0.699836562875046, 'f1-score': 0.8075661042427111, 'support': 165813}, 'accuracy': 0.7427922962797598, 'macro avg': {'precision': 0.7109195899728519, 'recall': 0.7936987692424011, 'f1-score': 0.7099265332169886, 'support': 215013}, 'weighted avg': {'precision': 0.8430245091328824, 'recall': 0.7427922962797598, 'f1-score': 0.762881672190086, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0:00:11.566662</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0:00:00.237343</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>BOW with (1-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.01, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -550,84 +714,166 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.9767470040614398</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.9189862938519996</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9340829571859726, 'recall': 0.7108333333333333, 'f1-score': 0.8073083182327074, 'support': 49200}, 'depression': {'precision': 0.9790942660951522, 'recall': 0.9963096541123133, 'f1-score': 0.9876269451709513, 'support': 668772}, 'accuracy': 0.9767470040614398, 'macro avg': {'precision': 0.9565886116405624, 'recall': 0.8535714937228234, 'f1-score': 0.8974676317018293, 'support': 717972}, 'weighted avg': {'precision': 0.9760098054221291, 'recall': 0.9767470040614398, 'f1-score': 0.9752703679710584, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9807000030250779, 'recall': 0.6589227642276423, 'f1-score': 0.7882368673790681, 'support': 49200}, 'depression': {'precision': 0.9077744069994944, 'recall': 0.996152292039828, 'f1-score': 0.9499121543323298, 'support': 165813}, 'accuracy': 0.9189862938519996, 'macro avg': {'precision': 0.9442372050122861, 'recall': 0.8275375281337352, 'f1-score': 0.869074510855699, 'support': 215013}, 'weighted avg': {'precision': 0.9244614878944111, 'recall': 0.9189862938519996, 'f1-score': 0.9129170697648827, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0:00:25.105664</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0:00:00.541459</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="C9" t="n">
+        <v>0.9764405854267297</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9174189467613586</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9357302885523794, 'recall': 0.7045934959349593, 'f1-score': 0.8038772363096688, 'support': 49200}, 'depression': {'precision': 0.9786555053787128, 'recall': 0.996439743290688, 'f1-score': 0.9874675575332834, 'support': 668772}, 'accuracy': 0.9764405854267297, 'macro avg': {'precision': 0.9571928969655461, 'recall': 0.8505166196128237, 'f1-score': 0.8956723969214762, 'support': 717972}, 'weighted avg': {'precision': 0.9757139969802578, 'recall': 0.9764405854267297, 'f1-score': 0.9748867830682599, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9813250061229488, 'recall': 0.6515040650406504, 'f1-score': 0.7831036841590931, 'support': 49200}, 'depression': {'precision': 0.9059715161585751, 'recall': 0.9963211569659798, 'f1-score': 0.9490007525232508, 'support': 165813}, 'accuracy': 0.9174189467613586, 'macro avg': {'precision': 0.943648261140762, 'recall': 0.823912611003315, 'f1-score': 0.866052218341172, 'support': 215013}, 'weighted avg': {'precision': 0.9232141559349941, 'recall': 0.9174189467613586, 'f1-score': 0.9110396256913079, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0:00:21.842818</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0:00:00.532575</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>BOW with (1-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>MultinomialNB(alpha=0.1, class_prior=None, fit_prior=True)</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C10" t="n">
         <v>0.9308078866585326</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D10" t="n">
         <v>0.8271639389246231</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.49267230806965906, 'recall': 0.32660569105691056, 'f1-score': 0.3928082526645155, 'support': 49200}, 'depression': {'precision': 0.9516587000040855, 'recall': 0.9752576363842984, 'f1-score': 0.9633136601562038, 'support': 668772}, 'accuracy': 0.9308078866585326, 'macro avg': {'precision': 0.7221655040368723, 'recall': 0.6509316637206045, 'f1-score': 0.6780609564103597, 'support': 717972}, 'weighted avg': {'precision': 0.920206038224554, 'recall': 0.9308078866585326, 'f1-score': 0.9242190073722636, 'support': 717972}}</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.799452736318408, 'recall': 0.32660569105691056, 'f1-score': 0.4637518037518038, 'support': 49200}, 'depression': {'precision': 0.8300215993802363, 'recall': 0.9756894815243679, 'f1-score': 0.8969799792640397, 'support': 165813}, 'accuracy': 0.8271639389246231, 'macro avg': {'precision': 0.8147371678493222, 'recall': 0.6511475862906392, 'f1-score': 0.6803658915079218, 'support': 215013}, 'weighted avg': {'precision': 0.8230267290112729, 'recall': 0.8271639389246231, 'f1-score': 0.7978472466608855, 'support': 215013}}</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0:00:03.603629</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0:00:00.041397</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0:00:02.704765</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0:00:00.037899</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>BOW with (2-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8666298964305015</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.899140982173171</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.32597969588684717, 'recall': 0.886280487804878, 'f1-score': 0.47664593421728624, 'support': 49200}, 'depression': {'precision': 0.9904228987720085, 'recall': 0.8651842481443601, 'f1-score': 0.923577269513112, 'support': 668772}, 'accuracy': 0.8666298964305015, 'macro avg': {'precision': 0.6582012973294278, 'recall': 0.8757323679746191, 'f1-score': 0.7001116018651992, 'support': 717972}, 'weighted avg': {'precision': 0.9448910318162638, 'recall': 0.8666298964305015, 'f1-score': 0.8929506967546277, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.7304509514875368, 'recall': 0.886280487804878, 'f1-score': 0.8008558624742874, 'support': 49200}, 'depression': {'precision': 0.9639768988584636, 'recall': 0.9029569454747215, 'f1-score': 0.9324697163142652, 'support': 165813}, 'accuracy': 0.899140982173171, 'macro avg': {'precision': 0.8472139251730002, 'recall': 0.8946187166397997, 'f1-score': 0.8666627893942763, 'support': 215013}, 'weighted avg': {'precision': 0.9105407037881673, 'recall': 0.899140982173171, 'f1-score': 0.902353390283156, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0:00:02.677838</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0:00:00.036902</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>BOW with (2-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=0.1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.6962917773952187</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.7708975736350825</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.17255288286261702, 'recall': 0.9042682926829269, 'f1-score': 0.2898050378785411, 'support': 49200}, 'depression': {'precision': 0.9897639403831024, 'recall': 0.6809914290670064, 'f1-score': 0.8068455412743265, 'support': 668772}, 'accuracy': 0.6962917773952187, 'macro avg': {'precision': 0.5811584116228597, 'recall': 0.7926298608749667, 'f1-score': 0.5483252895764338, 'support': 717972}, 'weighted avg': {'precision': 0.9337634500714915, 'recall': 0.6962917773952187, 'f1-score': 0.7714146431793136, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.4996630727762803, 'recall': 0.9042682926829269, 'f1-score': 0.6436631944444444, 'support': 49200}, 'depression': {'precision': 0.9626110356981258, 'recall': 0.7313238407121275, 'f1-score': 0.8311776438897, 'support': 165813}, 'accuracy': 0.7708975736350825, 'macro avg': {'precision': 0.7311370542372031, 'recall': 0.8177960666975272, 'f1-score': 0.7374204191670721, 'support': 215013}, 'weighted avg': {'precision': 0.8566777210810803, 'recall': 0.7708975736350825, 'f1-score': 0.7882699549931841, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0:00:04.095732</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0:00:00.080805</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>BOW with (2-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.001, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -637,84 +883,166 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0.9442137019270946</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8199411198392655</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.8361137649739104, 'recall': 0.23123983739837398, 'f1-score': 0.3622844587386756, 'support': 49200}, 'depression': {'precision': 0.946301988315717, 'recall': 0.9966655302554532, 'f1-score': 0.9708310241439855, 'support': 668772}, 'accuracy': 0.9442137019270946, 'macro avg': {'precision': 0.8912078766448137, 'recall': 0.6139526838269136, 'f1-score': 0.6665577414413305, 'support': 717972}, 'weighted avg': {'precision': 0.9387511916433998, 'recall': 0.9442137019270946, 'f1-score': 0.929129549688239, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9222034307803817, 'recall': 0.2327439024390244, 'f1-score': 0.3716831393933493, 'support': 49200}, 'depression': {'precision': 0.8136735177397382, 'recall': 0.9941741600477646, 'f1-score': 0.8949129907249822, 'support': 165813}, 'accuracy': 0.8199411198392655, 'macro avg': {'precision': 0.86793847426006, 'recall': 0.6134590312433945, 'f1-score': 0.6332980650591657, 'support': 215013}, 'weighted avg': {'precision': 0.8385076985641519, 'recall': 0.8199411198392655, 'f1-score': 0.7751857710428405, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>0:00:14.739498</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0:00:00.185483</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="C13" t="n">
+        <v>0.9441760960037439</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.819982977773437</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.8373779224622669, 'recall': 0.23004065040650407, 'f1-score': 0.36092863065246505, 'support': 49200}, 'depression': {'precision': 0.946225172331558, 'recall': 0.9967133791486485, 'f1-score': 0.9708132953886753, 'support': 668772}, 'accuracy': 0.9441760960037439, 'macro avg': {'precision': 0.8918015473969125, 'recall': 0.6133770147775763, 'f1-score': 0.6658709630205701, 'support': 717972}, 'weighted avg': {'precision': 0.9387662676757091, 'recall': 0.9441760960037439, 'f1-score': 0.9290201258708924, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9245145631067961, 'recall': 0.23225609756097562, 'f1-score': 0.37124756335282655, 'support': 49200}, 'depression': {'precision': 0.813607496558156, 'recall': 0.9943731794250149, 'f1-score': 0.8949536727947761, 'support': 165813}, 'accuracy': 0.819982977773437, 'macro avg': {'precision': 0.8690610298324761, 'recall': 0.6133146384929953, 'f1-score': 0.6331006180738014, 'support': 215013}, 'weighted avg': {'precision': 0.8389856256675267, 'recall': 0.819982977773437, 'f1-score': 0.775117474125189, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0:00:13.036273</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0:00:00.174533</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>BOW with (2-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>MultinomialNB(alpha=0.1, class_prior=None, fit_prior=True)</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C14" t="n">
         <v>0.9684235596931356</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D14" t="n">
         <v>0.8997548985410184</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.9472033984019419, 'recall': 0.5710365853658537, 'f1-score': 0.7125194963289838, 'support': 49200}, 'depression': {'precision': 0.9693379882059128, 'recall': 0.9976583947892556, 'f1-score': 0.9832943158229821, 'support': 668772}, 'accuracy': 0.9684235596931356, 'macro avg': {'precision': 0.9582706933039273, 'recall': 0.7843474900775547, 'f1-score': 0.847906906075983, 'support': 717972}, 'weighted avg': {'precision': 0.9678211855752318, 'recall': 0.9684235596931356, 'f1-score': 0.9647391059831768, 'support': 717972}}</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.984269899103139, 'recall': 0.5710365853658537, 'f1-score': 0.7227567400699733, 'support': 49200}, 'depression': {'precision': 0.8868176479736578, 'recall': 0.9972921302913523, 'f1-score': 0.9388160621320418, 'support': 165813}, 'accuracy': 0.8997548985410184, 'macro avg': {'precision': 0.9355437735383985, 'recall': 0.784164357828603, 'f1-score': 0.8307864011010075, 'support': 215013}, 'weighted avg': {'precision': 0.9091170008293944, 'recall': 0.8997548985410184, 'f1-score': 0.8893766391880629, 'support': 215013}}</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0:00:06.318381</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0:00:00.046896</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0:00:06.129788</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0:00:00.044858</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>TFIDF with (1-1) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9596669508003097</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9426825354745992</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.653567201772221, 'recall': 0.8754878048780488, 'f1-score': 0.748423192535576, 'support': 49200}, 'depression': {'precision': 0.9906052454812856, 'recall': 0.9658598147051611, 'f1-score': 0.9780760396051598, 'support': 668772}, 'accuracy': 0.9596669508003097, 'macro avg': {'precision': 0.8220862236267533, 'recall': 0.920673809791605, 'f1-score': 0.8632496160703679, 'support': 717972}, 'weighted avg': {'precision': 0.9675092587986768, 'recall': 0.9596669508003097, 'f1-score': 0.9623387684082001, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.874208475401851, 'recall': 0.8754878048780488, 'f1-score': 0.8748476724348037, 'support': 49200}, 'depression': {'precision': 0.9630387170344091, 'recall': 0.9626205424182663, 'f1-score': 0.9628295843211062, 'support': 165813}, 'accuracy': 0.9426825354745992, 'macro avg': {'precision': 0.9186235962181301, 'recall': 0.9190541736481576, 'f1-score': 0.9188386283779549, 'support': 215013}, 'weighted avg': {'precision': 0.9427122814778528, 'recall': 0.9426825354745992, 'f1-score': 0.9426972664389034, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0:00:05.467803</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0:00:00.041888</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>TFIDF with (1-1) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.6912205489907685</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.7550427183472628</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.1673410036757474, 'recall': 0.8818292682926829, 'f1-score': 0.28130075502403823, 'support': 49200}, 'depression': {'precision': 0.9873251872118246, 'recall': 0.6771979090033674, 'f1-score': 0.8033707117750518, 'support': 668772}, 'accuracy': 0.6912205489907685, 'macro avg': {'precision': 0.577333095443786, 'recall': 0.7795135886480251, 'f1-score': 0.542335733399545, 'support': 717972}, 'weighted avg': {'precision': 0.9311346646984466, 'recall': 0.6912205489907685, 'f1-score': 0.7675951636030481, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.48077924668387984, 'recall': 0.8818292682926829, 'f1-score': 0.6222846938848688, 'support': 49200}, 'depression': {'precision': 0.9534030070849229, 'recall': 0.7174226387557068, 'f1-score': 0.8187483868747527, 'support': 165813}, 'accuracy': 0.7550427183472628, 'macro avg': {'precision': 0.7170911268844014, 'recall': 0.7996259535241949, 'f1-score': 0.7205165403798108, 'support': 215013}, 'weighted avg': {'precision': 0.8452556438476706, 'recall': 0.7550427183472628, 'f1-score': 0.7737929018803463, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0:00:09.092702</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0:00:00.158599</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>TFIDF with (1-1) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.01, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -724,84 +1052,166 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0.9823266088371134</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.9376595833740285</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.932441075447116, 'recall': 0.8000609756097561, 'f1-score': 0.8611934584039819, 'support': 49200}, 'depression': {'precision': 0.9854429920814731, 'recall': 0.9957354673939699, 'f1-score': 0.9905624943753539, 'support': 668772}, 'accuracy': 0.9823266088371134, 'macro avg': {'precision': 0.9589420337642945, 'recall': 0.8978982215018629, 'f1-score': 0.9258779763896678, 'support': 717972}, 'weighted avg': {'precision': 0.981810964233019, 'recall': 0.9823266088371134, 'f1-score': 0.9816973066385182, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9825819672131147, 'recall': 0.7406910569105691, 'f1-score': 0.8446597441127388, 'support': 49200}, 'depression': {'precision': 0.9282956301812562, 'recall': 0.9961040449180704, 'f1-score': 0.961005184180975, 'support': 165813}, 'accuracy': 0.9376595833740285, 'macro avg': {'precision': 0.9554387986971855, 'recall': 0.8683975509143198, 'f1-score': 0.9028324641468569, 'support': 215013}, 'weighted avg': {'precision': 0.9407176129542395, 'recall': 0.9376595833740285, 'f1-score': 0.9343826280966581, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0:00:29.216584</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0:00:00.357652</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="C17" t="n">
+        <v>0.9824422122311176</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9390827531358569</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9305987009319401, 'recall': 0.8037195121951219, 'f1-score': 0.8625179950268289, 'support': 49200}, 'depression': {'precision': 0.9857034997335228, 'recall': 0.9955904254364716, 'f1-score': 0.9906222940341542, 'support': 668772}, 'accuracy': 0.9824422122311176, 'macro avg': {'precision': 0.9581511003327314, 'recall': 0.8996549688157968, 'f1-score': 0.9265701445304916, 'support': 717972}, 'weighted avg': {'precision': 0.9819273690473151, 'recall': 0.9824422122311176, 'f1-score': 0.9818437741041841, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9820799059929495, 'recall': 0.7474186991869919, 'f1-score': 0.8488296939199483, 'support': 49200}, 'depression': {'precision': 0.9300159374665623, 'recall': 0.9959532726625777, 'f1-score': 0.9618558922715809, 'support': 165813}, 'accuracy': 0.9390827531358569, 'macro avg': {'precision': 0.956047921729756, 'recall': 0.8716859859247847, 'f1-score': 0.9053427930957646, 'support': 215013}, 'weighted avg': {'precision': 0.9419293903810292, 'recall': 0.9390827531358569, 'f1-score': 0.935992856274221, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0:00:23.371794</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0:00:00.336078</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>TFIDF with (1-1) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>MultinomialNB(alpha=0.1, class_prior=None, fit_prior=True)</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C18" t="n">
         <v>0.965383051149627</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D18" t="n">
         <v>0.8906019636022008</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.9356836077308518, 'recall': 0.5313617886178862, 'f1-score': 0.67780658542909, 'support': 49200}, 'depression': {'precision': 0.9665856076239943, 'recall': 0.997312985591502, 'f1-score': 0.9817089146043139, 'support': 668772}, 'accuracy': 0.965383051149627, 'macro avg': {'precision': 0.951134607677423, 'recall': 0.7643373871046941, 'f1-score': 0.8297577500167019, 'support': 717972}, 'weighted avg': {'precision': 0.9644680063878142, 'recall': 0.965383051149627, 'f1-score': 0.9608835974674046, 'support': 717972}}</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.9825240529164161, 'recall': 0.5313617886178862, 'f1-score': 0.6897161249472351, 'support': 49200}, 'depression': {'precision': 0.8776200207000876, 'recall': 0.997195636047837, 'f1-score': 0.9335945660581901, 'support': 165813}, 'accuracy': 0.8906019636022008, 'macro avg': {'precision': 0.9300720368082518, 'recall': 0.7642787123328616, 'f1-score': 0.8116553455027127, 'support': 215013}, 'weighted avg': {'precision': 0.9016245152424797, 'recall': 0.8906019636022008, 'f1-score': 0.8777894784464689, 'support': 215013}}</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0:00:08.382444</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0:00:00.058822</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0:00:07.494058</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0:00:00.055850</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>TFIDF with (1-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9529145983408823</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.9419569979489613</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.607039550536797, 'recall': 0.8872154471544715, 'f1-score': 0.7208607193579285, 'support': 49200}, 'depression': {'precision': 0.9914110676341663, 'recall': 0.9577479320306472, 'f1-score': 0.9742888086422945, 'support': 668772}, 'accuracy': 0.9529145983408823, 'macro avg': {'precision': 0.7992253090854817, 'recall': 0.9224816895925594, 'f1-score': 0.8475747640001114, 'support': 717972}, 'weighted avg': {'precision': 0.9650714908244988, 'recall': 0.9529145983408823, 'f1-score': 0.9569223068946068, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.8629749713336761, 'recall': 0.8872154471544715, 'f1-score': 0.8749273416046982, 'support': 49200}, 'depression': {'precision': 0.9662533220621415, 'recall': 0.9581998998872223, 'f1-score': 0.9622097600562007, 'support': 165813}, 'accuracy': 0.9419569979489613, 'macro avg': {'precision': 0.9146141466979087, 'recall': 0.9227076735208469, 'f1-score': 0.9185685508304495, 'support': 215013}, 'weighted avg': {'precision': 0.9426208214419907, 'recall': 0.9419569979489613, 'f1-score': 0.9422375026214692, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0:00:07.997329</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0:00:00.055851</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>TFIDF with (1-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=0.1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.6761196815474698</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.7427922962797598</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.16133120037831628, 'recall': 0.8875609756097561, 'f1-score': 0.2730333601147955, 'support': 49200}, 'depression': {'precision': 0.9876324337859016, 'recall': 0.660564437506355, 'f1-score': 0.791646767992359, 'support': 668772}, 'accuracy': 0.6761196815474698, 'macro avg': {'precision': 0.5744818170821089, 'recall': 0.7740627065580555, 'f1-score': 0.5323400640535773, 'support': 717972}, 'weighted avg': {'precision': 0.9310090269070076, 'recall': 0.6761196815474698, 'f1-score': 0.7561080844955428, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.46734233029034983, 'recall': 0.8875609756097561, 'f1-score': 0.6122869621912661, 'support': 49200}, 'depression': {'precision': 0.954496849655354, 'recall': 0.699836562875046, 'f1-score': 0.8075661042427111, 'support': 165813}, 'accuracy': 0.7427922962797598, 'macro avg': {'precision': 0.7109195899728519, 'recall': 0.7936987692424011, 'f1-score': 0.7099265332169886, 'support': 215013}, 'weighted avg': {'precision': 0.8430245091328824, 'recall': 0.7427922962797598, 'f1-score': 0.762881672190086, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0:00:11.839052</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0:00:00.204453</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>TFIDF with (1-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.01, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -811,84 +1221,166 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.9809045478096639</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.9351667108500417</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9213363092411435, 'recall': 0.7886788617886179, 'f1-score': 0.8498620176091813, 'support': 49200}, 'depression': {'precision': 0.9846165455363273, 'recall': 0.9950461442763752, 'f1-score': 0.9898038714053256, 'support': 668772}, 'accuracy': 0.9809045478096639, 'macro avg': {'precision': 0.9529764273887353, 'recall': 0.8918625030324965, 'f1-score': 0.9198329445072535, 'support': 717972}, 'weighted avg': {'precision': 0.9802801819654317, 'recall': 0.9809045478096639, 'f1-score': 0.9802141670620221, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9799629750626156, 'recall': 0.7316260162601625, 'f1-score': 0.8377787087464507, 'support': 49200}, 'depression': {'precision': 0.9259371441712801, 'recall': 0.9955612647982969, 'f1-score': 0.9594878143763041, 'support': 165813}, 'accuracy': 0.9351667108500417, 'macro avg': {'precision': 0.9529500596169479, 'recall': 0.8635936405292297, 'f1-score': 0.8986332615613775, 'support': 215013}, 'weighted avg': {'precision': 0.9382995170503792, 'recall': 0.9351667108500417, 'f1-score': 0.9316379262440109, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0:00:28.961622</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0:00:00.545843</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="C21" t="n">
+        <v>0.980872513134217</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.9352225214289368</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9198569974193243, 'recall': 0.7896747967479675, 'f1-score': 0.8498091582182268, 'support': 49200}, 'depression': {'precision': 0.9846863045424612, 'recall': 0.9949384842666859, 'f1-score': 0.9897858471543844, 'support': 668772}, 'accuracy': 0.980872513134217, 'macro avg': {'precision': 0.9522716509808927, 'recall': 0.8923066405073267, 'f1-score': 0.9197975026863057, 'support': 717972}, 'weighted avg': {'precision': 0.9802437888030475, 'recall': 0.980872513134217, 'f1-score': 0.9801937556861114, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9791089377886444, 'recall': 0.7325406504065041, 'f1-score': 0.8380653412393908, 'support': 49200}, 'depression': {'precision': 0.9261572476333171, 'recall': 0.9953622454210466, 'f1-score': 0.9595135109994885, 'support': 165813}, 'accuracy': 0.9352225214289368, 'macro avg': {'precision': 0.9526330927109807, 'recall': 0.8639514479137753, 'f1-score': 0.8987894261194396, 'support': 215013}, 'weighted avg': {'precision': 0.9382738320056206, 'recall': 0.9352225214289368, 'f1-score': 0.9317233310931721, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0:00:21.555165</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0:00:00.440821</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>TFIDF with (1-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>MultinomialNB(alpha=0.1, class_prior=None, fit_prior=True)</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C22" t="n">
         <v>0.938141041711933</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D22" t="n">
         <v>0.7961890676377708</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.8825315646475947, 'recall': 0.11223577235772357, 'f1-score': 0.19914528373334298, 'support': 49200}, 'depression': {'precision': 0.9386299291148845, 'recall': 0.9989009707344207, 'f1-score': 0.9678280201117432, 'support': 668772}, 'accuracy': 0.938141041711933, 'macro avg': {'precision': 0.9105807468812397, 'recall': 0.5555683715460722, 'f1-score': 0.5834866519225431, 'support': 717972}, 'weighted avg': {'precision': 0.9347857130008986, 'recall': 0.938141041711933, 'f1-score': 0.9151529984816277, 'support': 717972}}</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>{'non-depression': {'precision': 0.9745852453229792, 'recall': 0.11223577235772357, 'f1-score': 0.20129041665147815, 'support': 49200}, 'depression': {'precision': 0.7913607551099371, 'recall': 0.9991315518083624, 'f1-score': 0.8831911717667128, 'support': 165813}, 'accuracy': 0.7961890676377708, 'macro avg': {'precision': 0.8829730002164582, 'recall': 0.555683662083043, 'f1-score': 0.5422407942090954, 'support': 215013}, 'weighted avg': {'precision': 0.8332868010628873, 'recall': 0.7961890676377708, 'f1-score': 0.7271563406092035, 'support': 215013}}</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>0:00:03.776537</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>0:00:00.026929</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0:00:02.702394</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0:00:00.023936</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>TFIDF with (2-2) n-grams</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ComplementNB(alpha=0.1, class_prior=None, fit_prior=True, norm=False)</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.8773336564657117</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.9077497639677601</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.34544702710869724, 'recall': 0.8829471544715447, 'f1-score': 0.49660194452224315, 'support': 49200}, 'depression': {'precision': 0.9902755568463694, 'recall': 0.8769206844784172, 'f1-score': 0.9301573127801863, 'support': 668772}, 'accuracy': 0.8773336564657117, 'macro avg': {'precision': 0.6678612919775333, 'recall': 0.8799339194749809, 'f1-score': 0.7133796286512147, 'support': 717972}, 'weighted avg': {'precision': 0.9460878118325059, 'recall': 0.8773336564657117, 'f1-score': 0.9004473462100544, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.7552723542604796, 'recall': 0.8829471544715447, 'f1-score': 0.814134580244947, 'support': 49200}, 'depression': {'precision': 0.9634339919743994, 'recall': 0.9151091892674278, 'f1-score': 0.9386500221150664, 'support': 165813}, 'accuracy': 0.9077497639677601, 'macro avg': {'precision': 0.8593531731174395, 'recall': 0.8990281718694862, 'f1-score': 0.8763923011800068, 'support': 215013}, 'weighted avg': {'precision': 0.9158017438055682, 'recall': 0.9077497639677601, 'f1-score': 0.9101579786571832, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0:00:02.632191</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0:00:00.020944</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>TFIDF with (2-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=0.1, binarize=0.0, class_prior=None, fit_prior=True)</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6962917773952187</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.7708975736350825</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.17255288286261702, 'recall': 0.9042682926829269, 'f1-score': 0.2898050378785411, 'support': 49200}, 'depression': {'precision': 0.9897639403831024, 'recall': 0.6809914290670064, 'f1-score': 0.8068455412743265, 'support': 668772}, 'accuracy': 0.6962917773952187, 'macro avg': {'precision': 0.5811584116228597, 'recall': 0.7926298608749667, 'f1-score': 0.5483252895764338, 'support': 717972}, 'weighted avg': {'precision': 0.9337634500714915, 'recall': 0.6962917773952187, 'f1-score': 0.7714146431793136, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.4996630727762803, 'recall': 0.9042682926829269, 'f1-score': 0.6436631944444444, 'support': 49200}, 'depression': {'precision': 0.9626110356981258, 'recall': 0.7313238407121275, 'f1-score': 0.8311776438897, 'support': 165813}, 'accuracy': 0.7708975736350825, 'macro avg': {'precision': 0.7311370542372031, 'recall': 0.8177960666975272, 'f1-score': 0.7374204191670721, 'support': 215013}, 'weighted avg': {'precision': 0.8566777210810803, 'recall': 0.7708975736350825, 'f1-score': 0.7882699549931841, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0:00:04.206755</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0:00:00.073802</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>TFIDF with (2-2) n-grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>SGDClassifier(alpha=0.01, average=False, class_weight=None,
               early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True,
@@ -898,33 +1390,33 @@
               validation_fraction=0.1, verbose=0, warm_start=False)</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>0.9479812583220516</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.825633798886579</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.8251042352424841, 'recall': 0.3056910569105691, 'f1-score': 0.446105475470131, 'support': 49200}, 'depression': {'precision': 0.9511821466136187, 'recall': 0.9952330540154193, 'f1-score': 0.9727091243361422, 'support': 668772}, 'accuracy': 0.9479812583220516, 'macro avg': {'precision': 0.8881431909280514, 'recall': 0.6504620554629942, 'f1-score': 0.7094072999031367, 'support': 717972}, 'weighted avg': {'precision': 0.9425424876304552, 'recall': 0.9479812583220516, 'f1-score': 0.9366228987950239, 'support': 717972}}</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>{'non-depression': {'precision': 0.9638697409080105, 'recall': 0.2472560975609756, 'f1-score': 0.3935555879070219, 'support': 49200}, 'depression': {'precision': 0.8170135183208822, 'recall': 0.9972499140598143, 'f1-score': 0.8981790035442212, 'support': 165813}, 'accuracy': 0.825633798886579, 'macro avg': {'precision': 0.8904416296144464, 'recall': 0.622253005810395, 'f1-score': 0.6458672957256215, 'support': 215013}, 'weighted avg': {'precision': 0.850617654588395, 'recall': 0.825633798886579, 'f1-score': 0.7827093712459405, 'support': 215013}}</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0:00:27.061738</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>0:00:00.165559</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
+      <c r="C25" t="n">
+        <v>0.9478405843124802</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.8249222140056648</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.8276362014163832, 'recall': 0.3016666666666667, 'f1-score': 0.44216704154439695, 'support': 49200}, 'depression': {'precision': 0.9509198773211207, 'recall': 0.9953780959729175, 'f1-score': 0.9726412192771683, 'support': 668772}, 'accuracy': 0.9478405843124802, 'macro avg': {'precision': 0.8892780393687519, 'recall': 0.6485223813197921, 'f1-score': 0.7074041304107826, 'support': 717972}, 'weighted avg': {'precision': 0.942471697093322, 'recall': 0.9478405843124802, 'f1-score': 0.9362897605232722, 'support': 717972}}</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>{'non-depression': {'precision': 0.9654422426292895, 'recall': 0.24359756097560975, 'f1-score': 0.3890349595871068, 'support': 49200}, 'depression': {'precision': 0.8163120252321088, 'recall': 0.9974127480957464, 'f1-score': 0.8978209178854109, 'support': 165813}, 'accuracy': 0.8249222140056648, 'macro avg': {'precision': 0.8908771339306991, 'recall': 0.6205051545356781, 'f1-score': 0.6434279387362588, 'support': 215013}, 'weighted avg': {'precision': 0.850436504663312, 'recall': 0.8249222140056648, 'f1-score': 0.7813987985332016, 'support': 215013}}</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0:00:16.306685</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0:00:00.144635</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>TFIDF with (2-2) n-grams</t>
         </is>

</xml_diff>